<commit_message>
Ajout axes courbe en s
</commit_message>
<xml_diff>
--- a/Gestion/Courbe_en_S.xlsx
+++ b/Gestion/Courbe_en_S.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,18 +434,18 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -498,7 +498,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -509,7 +509,9 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -562,7 +564,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -573,7 +575,9 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -626,7 +630,305 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -669,7 +971,9 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -733,7 +1037,9 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -797,7 +1103,9 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -861,6 +1169,235 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
@@ -890,33 +1427,26 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -942,502 +1472,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <border>
@@ -1445,40 +1479,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1995,6 +1995,64 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Date</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-CA" baseline="0"/>
+                  <a:t> (semaines)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2059,6 +2117,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Budget (heures)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2757,25 +2868,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:P7" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" headerRowBorderDxfId="33" tableBorderDxfId="34" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:P7" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
   <autoFilter ref="A1:P7"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="Semaine" dataDxfId="31" totalsRowDxfId="15"/>
-    <tableColumn id="2" name="W1" dataDxfId="30" totalsRowDxfId="14"/>
-    <tableColumn id="3" name="W2" dataDxfId="29" totalsRowDxfId="13"/>
-    <tableColumn id="4" name="W3" dataDxfId="28" totalsRowDxfId="12"/>
-    <tableColumn id="5" name="W4" dataDxfId="27" totalsRowDxfId="11"/>
-    <tableColumn id="6" name="W5" dataDxfId="26" totalsRowDxfId="10"/>
-    <tableColumn id="7" name="W6" dataDxfId="25" totalsRowDxfId="9"/>
-    <tableColumn id="8" name="W7" dataDxfId="24" totalsRowDxfId="8"/>
-    <tableColumn id="9" name="W8" dataDxfId="23" totalsRowDxfId="7"/>
-    <tableColumn id="10" name="W9" dataDxfId="22" totalsRowDxfId="6"/>
-    <tableColumn id="11" name="W10" dataDxfId="21" totalsRowDxfId="5"/>
-    <tableColumn id="12" name="W11" dataDxfId="20" totalsRowDxfId="4"/>
-    <tableColumn id="13" name="W12" dataDxfId="19" totalsRowDxfId="3"/>
-    <tableColumn id="14" name="W13" dataDxfId="18" totalsRowDxfId="2"/>
-    <tableColumn id="15" name="W14" dataDxfId="17" totalsRowDxfId="1"/>
-    <tableColumn id="16" name="W15" dataDxfId="16" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Semaine" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="2" name="W1" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="3" name="W2" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="4" name="W3" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="5" name="W4" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="6" name="W5" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="7" name="W6" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="8" name="W7" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="9" name="W8" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="10" name="W9" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="11" name="W10" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="12" name="W11" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="13" name="W12" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="14" name="W13" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="15" name="W14" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="16" name="W15" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3046,19 +3157,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1328125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="32.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="2"/>
-    <col min="3" max="3" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.109375" style="2"/>
+    <col min="2" max="2" width="10.1328125" style="2"/>
+    <col min="3" max="3" width="16.46484375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3108,7 +3219,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -3158,7 +3269,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
@@ -3200,7 +3311,7 @@
       <c r="O3" s="15"/>
       <c r="P3" s="16"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12" t="s">
         <v>21</v>
       </c>
@@ -3265,7 +3376,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
@@ -3330,7 +3441,7 @@
         <v>202.75</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="13" t="s">
         <v>23</v>
       </c>
@@ -3373,7 +3484,7 @@
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
     </row>
-    <row r="7" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -3426,7 +3537,7 @@
       <c r="O7" s="18"/>
       <c r="P7" s="18"/>
     </row>
-    <row r="8" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="19" t="s">
         <v>18</v>
       </c>
@@ -3438,7 +3549,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:16" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="19" t="s">
         <v>19</v>
       </c>
@@ -3450,7 +3561,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="3"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -3460,7 +3571,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="3"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -3470,7 +3581,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A12" s="3"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -3480,7 +3591,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -3490,7 +3601,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A14" s="3"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -3500,7 +3611,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="3"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -3510,7 +3621,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A16" s="3"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -3520,7 +3631,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A17" s="3"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -3530,7 +3641,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A18" s="3"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -3540,7 +3651,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A19" s="3"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -3550,7 +3661,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A20" s="3"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -3560,7 +3671,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="3"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -3570,7 +3681,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -3580,7 +3691,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A23" s="3"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3590,7 +3701,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A24" s="3"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -3600,7 +3711,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A25" s="3"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3610,7 +3721,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A26" s="3"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3620,7 +3731,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A27" s="3"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3630,7 +3741,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A28" s="3"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3640,7 +3751,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="3"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3650,7 +3761,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A30" s="3"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3660,7 +3771,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A31" s="3"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3670,7 +3781,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A32" s="3"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3680,7 +3791,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A33" s="3"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3690,7 +3801,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A34" s="3"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3700,7 +3811,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A35" s="3"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3710,7 +3821,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A36" s="3"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3720,7 +3831,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A37" s="3"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3730,7 +3841,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A38" s="3"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3740,7 +3851,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A39" s="3"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3750,7 +3861,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A40" s="3"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3760,7 +3871,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A41" s="3"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3770,7 +3881,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A42" s="3"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3780,7 +3891,7 @@
       <c r="G42" s="1"/>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A43" s="3"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3790,7 +3901,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A44" s="3"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3800,7 +3911,7 @@
       <c r="G44" s="1"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A45" s="3"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3810,7 +3921,7 @@
       <c r="G45" s="1"/>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A46" s="3"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3820,7 +3931,7 @@
       <c r="G46" s="1"/>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A47" s="3"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3830,7 +3941,7 @@
       <c r="G47" s="1"/>
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A48" s="3"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3840,7 +3951,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A49" s="3"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3850,7 +3961,7 @@
       <c r="G49" s="1"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A50" s="3"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3860,7 +3971,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A51" s="3"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3870,7 +3981,7 @@
       <c r="G51" s="1"/>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A52" s="3"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3880,7 +3991,7 @@
       <c r="G52" s="1"/>
       <c r="H52" s="4"/>
     </row>
-    <row r="53" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A53" s="3"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3890,7 +4001,7 @@
       <c r="G53" s="1"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A54" s="3"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3900,7 +4011,7 @@
       <c r="G54" s="1"/>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A55" s="3"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3910,7 +4021,7 @@
       <c r="G55" s="1"/>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A56" s="3"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3920,7 +4031,7 @@
       <c r="G56" s="1"/>
       <c r="H56" s="4"/>
     </row>
-    <row r="57" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A57" s="3"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3930,7 +4041,7 @@
       <c r="G57" s="1"/>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A58" s="3"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3940,7 +4051,7 @@
       <c r="G58" s="1"/>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A59" s="3"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3950,7 +4061,7 @@
       <c r="G59" s="1"/>
       <c r="H59" s="4"/>
     </row>
-    <row r="60" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A60" s="3"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3960,7 +4071,7 @@
       <c r="G60" s="1"/>
       <c r="H60" s="4"/>
     </row>
-    <row r="61" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A61" s="3"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3970,7 +4081,7 @@
       <c r="G61" s="1"/>
       <c r="H61" s="4"/>
     </row>
-    <row r="62" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A62" s="3"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3980,7 +4091,7 @@
       <c r="G62" s="1"/>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A63" s="3"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3990,7 +4101,7 @@
       <c r="G63" s="1"/>
       <c r="H63" s="4"/>
     </row>
-    <row r="64" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A64" s="3"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -4000,7 +4111,7 @@
       <c r="G64" s="1"/>
       <c r="H64" s="4"/>
     </row>
-    <row r="65" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A65" s="3"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -4010,7 +4121,7 @@
       <c r="G65" s="1"/>
       <c r="H65" s="4"/>
     </row>
-    <row r="66" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A66" s="3"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4020,7 +4131,7 @@
       <c r="G66" s="1"/>
       <c r="H66" s="4"/>
     </row>
-    <row r="67" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A67" s="3"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4030,7 +4141,7 @@
       <c r="G67" s="1"/>
       <c r="H67" s="4"/>
     </row>
-    <row r="68" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A68" s="3"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -4040,7 +4151,7 @@
       <c r="G68" s="1"/>
       <c r="H68" s="4"/>
     </row>
-    <row r="69" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A69" s="3"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -4050,7 +4161,7 @@
       <c r="G69" s="1"/>
       <c r="H69" s="4"/>
     </row>
-    <row r="70" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A70" s="3"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -4060,7 +4171,7 @@
       <c r="G70" s="1"/>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A71" s="3"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -4070,7 +4181,7 @@
       <c r="G71" s="1"/>
       <c r="H71" s="4"/>
     </row>
-    <row r="72" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A72" s="3"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -4080,7 +4191,7 @@
       <c r="G72" s="1"/>
       <c r="H72" s="4"/>
     </row>
-    <row r="73" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A73" s="3"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -4090,7 +4201,7 @@
       <c r="G73" s="1"/>
       <c r="H73" s="4"/>
     </row>
-    <row r="74" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A74" s="3"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4100,7 +4211,7 @@
       <c r="G74" s="1"/>
       <c r="H74" s="4"/>
     </row>
-    <row r="75" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A75" s="3"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -4110,7 +4221,7 @@
       <c r="G75" s="1"/>
       <c r="H75" s="4"/>
     </row>
-    <row r="76" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A76" s="3"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -4120,7 +4231,7 @@
       <c r="G76" s="1"/>
       <c r="H76" s="4"/>
     </row>
-    <row r="77" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A77" s="3"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -4130,7 +4241,7 @@
       <c r="G77" s="1"/>
       <c r="H77" s="4"/>
     </row>
-    <row r="78" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A78" s="3"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4140,7 +4251,7 @@
       <c r="G78" s="1"/>
       <c r="H78" s="4"/>
     </row>
-    <row r="79" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A79" s="3"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -4150,7 +4261,7 @@
       <c r="G79" s="1"/>
       <c r="H79" s="4"/>
     </row>
-    <row r="80" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A80" s="3"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -4160,7 +4271,7 @@
       <c r="G80" s="1"/>
       <c r="H80" s="4"/>
     </row>
-    <row r="81" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A81" s="3"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -4170,7 +4281,7 @@
       <c r="G81" s="1"/>
       <c r="H81" s="4"/>
     </row>
-    <row r="82" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A82" s="3"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -4180,7 +4291,7 @@
       <c r="G82" s="1"/>
       <c r="H82" s="4"/>
     </row>
-    <row r="83" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A83" s="3"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -4190,7 +4301,7 @@
       <c r="G83" s="1"/>
       <c r="H83" s="4"/>
     </row>
-    <row r="84" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A84" s="3"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -4200,7 +4311,7 @@
       <c r="G84" s="1"/>
       <c r="H84" s="4"/>
     </row>
-    <row r="85" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A85" s="3"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -4210,7 +4321,7 @@
       <c r="G85" s="1"/>
       <c r="H85" s="4"/>
     </row>
-    <row r="86" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A86" s="3"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -4220,7 +4331,7 @@
       <c r="G86" s="1"/>
       <c r="H86" s="4"/>
     </row>
-    <row r="87" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A87" s="3"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -4230,7 +4341,7 @@
       <c r="G87" s="1"/>
       <c r="H87" s="4"/>
     </row>
-    <row r="88" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A88" s="3"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -4240,7 +4351,7 @@
       <c r="G88" s="1"/>
       <c r="H88" s="4"/>
     </row>
-    <row r="89" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A89" s="3"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -4250,7 +4361,7 @@
       <c r="G89" s="1"/>
       <c r="H89" s="4"/>
     </row>
-    <row r="90" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A90" s="3"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -4260,7 +4371,7 @@
       <c r="G90" s="1"/>
       <c r="H90" s="4"/>
     </row>
-    <row r="91" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A91" s="3"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -4270,7 +4381,7 @@
       <c r="G91" s="1"/>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A92" s="3"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -4280,7 +4391,7 @@
       <c r="G92" s="1"/>
       <c r="H92" s="4"/>
     </row>
-    <row r="93" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A93" s="3"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -4290,7 +4401,7 @@
       <c r="G93" s="1"/>
       <c r="H93" s="4"/>
     </row>
-    <row r="94" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A94" s="3"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -4300,7 +4411,7 @@
       <c r="G94" s="1"/>
       <c r="H94" s="4"/>
     </row>
-    <row r="95" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A95" s="3"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -4310,7 +4421,7 @@
       <c r="G95" s="1"/>
       <c r="H95" s="4"/>
     </row>
-    <row r="96" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A96" s="3"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -4320,7 +4431,7 @@
       <c r="G96" s="1"/>
       <c r="H96" s="4"/>
     </row>
-    <row r="97" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A97" s="3"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -4330,7 +4441,7 @@
       <c r="G97" s="1"/>
       <c r="H97" s="4"/>
     </row>
-    <row r="98" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A98" s="3"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -4340,7 +4451,7 @@
       <c r="G98" s="1"/>
       <c r="H98" s="4"/>
     </row>
-    <row r="99" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A99" s="3"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -4350,7 +4461,7 @@
       <c r="G99" s="1"/>
       <c r="H99" s="4"/>
     </row>
-    <row r="100" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A100" s="3"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -4360,7 +4471,7 @@
       <c r="G100" s="1"/>
       <c r="H100" s="4"/>
     </row>
-    <row r="101" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A101" s="3"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -4370,7 +4481,7 @@
       <c r="G101" s="1"/>
       <c r="H101" s="4"/>
     </row>
-    <row r="102" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A102" s="3"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -4380,7 +4491,7 @@
       <c r="G102" s="1"/>
       <c r="H102" s="4"/>
     </row>
-    <row r="103" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A103" s="3"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -4390,7 +4501,7 @@
       <c r="G103" s="1"/>
       <c r="H103" s="4"/>
     </row>
-    <row r="104" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A104" s="3"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -4400,7 +4511,7 @@
       <c r="G104" s="1"/>
       <c r="H104" s="4"/>
     </row>
-    <row r="105" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A105" s="3"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -4410,7 +4521,7 @@
       <c r="G105" s="1"/>
       <c r="H105" s="4"/>
     </row>
-    <row r="106" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A106" s="3"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -4420,7 +4531,7 @@
       <c r="G106" s="1"/>
       <c r="H106" s="4"/>
     </row>
-    <row r="107" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A107" s="3"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -4430,7 +4541,7 @@
       <c r="G107" s="1"/>
       <c r="H107" s="4"/>
     </row>
-    <row r="108" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A108" s="3"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -4440,7 +4551,7 @@
       <c r="G108" s="1"/>
       <c r="H108" s="4"/>
     </row>
-    <row r="109" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A109" s="3"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -4450,7 +4561,7 @@
       <c r="G109" s="1"/>
       <c r="H109" s="4"/>
     </row>
-    <row r="110" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A110" s="3"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -4460,7 +4571,7 @@
       <c r="G110" s="1"/>
       <c r="H110" s="4"/>
     </row>
-    <row r="111" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A111" s="3"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -4470,7 +4581,7 @@
       <c r="G111" s="1"/>
       <c r="H111" s="4"/>
     </row>
-    <row r="112" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A112" s="3"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -4480,7 +4591,7 @@
       <c r="G112" s="1"/>
       <c r="H112" s="4"/>
     </row>
-    <row r="113" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A113" s="3"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -4490,7 +4601,7 @@
       <c r="G113" s="1"/>
       <c r="H113" s="4"/>
     </row>
-    <row r="114" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A114" s="3"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -4500,7 +4611,7 @@
       <c r="G114" s="1"/>
       <c r="H114" s="4"/>
     </row>
-    <row r="115" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A115" s="3"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -4510,7 +4621,7 @@
       <c r="G115" s="1"/>
       <c r="H115" s="4"/>
     </row>
-    <row r="116" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A116" s="3"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -4520,7 +4631,7 @@
       <c r="G116" s="1"/>
       <c r="H116" s="4"/>
     </row>
-    <row r="117" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A117" s="3"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -4530,7 +4641,7 @@
       <c r="G117" s="1"/>
       <c r="H117" s="4"/>
     </row>
-    <row r="118" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A118" s="3"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -4540,7 +4651,7 @@
       <c r="G118" s="1"/>
       <c r="H118" s="4"/>
     </row>
-    <row r="119" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A119" s="3"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -4550,7 +4661,7 @@
       <c r="G119" s="1"/>
       <c r="H119" s="4"/>
     </row>
-    <row r="120" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A120" s="3"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -4560,7 +4671,7 @@
       <c r="G120" s="1"/>
       <c r="H120" s="4"/>
     </row>
-    <row r="121" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A121" s="3"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -4570,7 +4681,7 @@
       <c r="G121" s="1"/>
       <c r="H121" s="4"/>
     </row>
-    <row r="122" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A122" s="3"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -4580,7 +4691,7 @@
       <c r="G122" s="1"/>
       <c r="H122" s="4"/>
     </row>
-    <row r="123" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A123" s="3"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -4590,7 +4701,7 @@
       <c r="G123" s="1"/>
       <c r="H123" s="4"/>
     </row>
-    <row r="124" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A124" s="3"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -4600,7 +4711,7 @@
       <c r="G124" s="1"/>
       <c r="H124" s="4"/>
     </row>
-    <row r="125" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A125" s="3"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -4610,7 +4721,7 @@
       <c r="G125" s="1"/>
       <c r="H125" s="4"/>
     </row>
-    <row r="126" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A126" s="3"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -4620,7 +4731,7 @@
       <c r="G126" s="1"/>
       <c r="H126" s="4"/>
     </row>
-    <row r="127" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A127" s="3"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -4630,7 +4741,7 @@
       <c r="G127" s="1"/>
       <c r="H127" s="4"/>
     </row>
-    <row r="128" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A128" s="3"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -4640,7 +4751,7 @@
       <c r="G128" s="1"/>
       <c r="H128" s="4"/>
     </row>
-    <row r="129" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A129" s="3"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -4650,7 +4761,7 @@
       <c r="G129" s="1"/>
       <c r="H129" s="4"/>
     </row>
-    <row r="130" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A130" s="3"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -4660,7 +4771,7 @@
       <c r="G130" s="1"/>
       <c r="H130" s="4"/>
     </row>
-    <row r="131" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A131" s="3"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -4670,7 +4781,7 @@
       <c r="G131" s="1"/>
       <c r="H131" s="4"/>
     </row>
-    <row r="132" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A132" s="3"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -4680,7 +4791,7 @@
       <c r="G132" s="1"/>
       <c r="H132" s="4"/>
     </row>
-    <row r="133" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A133" s="3"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -4690,7 +4801,7 @@
       <c r="G133" s="1"/>
       <c r="H133" s="4"/>
     </row>
-    <row r="134" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A134" s="3"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -4700,7 +4811,7 @@
       <c r="G134" s="1"/>
       <c r="H134" s="4"/>
     </row>
-    <row r="135" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A135" s="3"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -4710,7 +4821,7 @@
       <c r="G135" s="1"/>
       <c r="H135" s="4"/>
     </row>
-    <row r="136" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A136" s="3"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -4720,7 +4831,7 @@
       <c r="G136" s="1"/>
       <c r="H136" s="4"/>
     </row>
-    <row r="137" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A137" s="3"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -4730,7 +4841,7 @@
       <c r="G137" s="1"/>
       <c r="H137" s="4"/>
     </row>
-    <row r="138" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A138" s="3"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -4740,7 +4851,7 @@
       <c r="G138" s="1"/>
       <c r="H138" s="4"/>
     </row>
-    <row r="139" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A139" s="3"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -4750,7 +4861,7 @@
       <c r="G139" s="1"/>
       <c r="H139" s="4"/>
     </row>
-    <row r="140" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A140" s="3"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -4760,7 +4871,7 @@
       <c r="G140" s="1"/>
       <c r="H140" s="4"/>
     </row>
-    <row r="141" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A141" s="3"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -4770,7 +4881,7 @@
       <c r="G141" s="1"/>
       <c r="H141" s="4"/>
     </row>
-    <row r="142" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A142" s="3"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -4780,7 +4891,7 @@
       <c r="G142" s="1"/>
       <c r="H142" s="4"/>
     </row>
-    <row r="143" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A143" s="3"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -4790,7 +4901,7 @@
       <c r="G143" s="1"/>
       <c r="H143" s="4"/>
     </row>
-    <row r="144" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A144" s="3"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -4800,7 +4911,7 @@
       <c r="G144" s="1"/>
       <c r="H144" s="4"/>
     </row>
-    <row r="145" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A145" s="3"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -4810,7 +4921,7 @@
       <c r="G145" s="1"/>
       <c r="H145" s="4"/>
     </row>
-    <row r="146" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A146" s="3"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -4820,7 +4931,7 @@
       <c r="G146" s="1"/>
       <c r="H146" s="4"/>
     </row>
-    <row r="147" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A147" s="3"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -4830,7 +4941,7 @@
       <c r="G147" s="1"/>
       <c r="H147" s="4"/>
     </row>
-    <row r="148" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A148" s="3"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -4840,7 +4951,7 @@
       <c r="G148" s="1"/>
       <c r="H148" s="4"/>
     </row>
-    <row r="149" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A149" s="3"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -4850,7 +4961,7 @@
       <c r="G149" s="1"/>
       <c r="H149" s="4"/>
     </row>
-    <row r="150" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A150" s="3"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -4860,7 +4971,7 @@
       <c r="G150" s="1"/>
       <c r="H150" s="4"/>
     </row>
-    <row r="151" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A151" s="3"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -4870,7 +4981,7 @@
       <c r="G151" s="1"/>
       <c r="H151" s="4"/>
     </row>
-    <row r="152" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A152" s="3"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -4880,7 +4991,7 @@
       <c r="G152" s="1"/>
       <c r="H152" s="4"/>
     </row>
-    <row r="153" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A153" s="3"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -4890,7 +5001,7 @@
       <c r="G153" s="1"/>
       <c r="H153" s="4"/>
     </row>
-    <row r="154" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A154" s="3"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -4900,7 +5011,7 @@
       <c r="G154" s="1"/>
       <c r="H154" s="4"/>
     </row>
-    <row r="155" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A155" s="3"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -4910,7 +5021,7 @@
       <c r="G155" s="1"/>
       <c r="H155" s="4"/>
     </row>
-    <row r="156" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A156" s="3"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4920,7 +5031,7 @@
       <c r="G156" s="1"/>
       <c r="H156" s="4"/>
     </row>
-    <row r="157" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A157" s="3"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -4930,7 +5041,7 @@
       <c r="G157" s="1"/>
       <c r="H157" s="4"/>
     </row>
-    <row r="158" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A158" s="3"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4940,7 +5051,7 @@
       <c r="G158" s="1"/>
       <c r="H158" s="4"/>
     </row>
-    <row r="159" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A159" s="3"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -4950,7 +5061,7 @@
       <c r="G159" s="1"/>
       <c r="H159" s="4"/>
     </row>
-    <row r="160" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A160" s="3"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -4960,7 +5071,7 @@
       <c r="G160" s="1"/>
       <c r="H160" s="4"/>
     </row>
-    <row r="161" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A161" s="3"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -4970,7 +5081,7 @@
       <c r="G161" s="1"/>
       <c r="H161" s="4"/>
     </row>
-    <row r="162" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A162" s="3"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -4980,7 +5091,7 @@
       <c r="G162" s="1"/>
       <c r="H162" s="4"/>
     </row>
-    <row r="163" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A163" s="3"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -4990,7 +5101,7 @@
       <c r="G163" s="1"/>
       <c r="H163" s="4"/>
     </row>
-    <row r="164" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A164" s="3"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -5000,7 +5111,7 @@
       <c r="G164" s="1"/>
       <c r="H164" s="4"/>
     </row>
-    <row r="165" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A165" s="3"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -5010,7 +5121,7 @@
       <c r="G165" s="1"/>
       <c r="H165" s="4"/>
     </row>
-    <row r="166" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A166" s="3"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -5020,7 +5131,7 @@
       <c r="G166" s="1"/>
       <c r="H166" s="4"/>
     </row>
-    <row r="167" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A167" s="3"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -5030,7 +5141,7 @@
       <c r="G167" s="1"/>
       <c r="H167" s="4"/>
     </row>
-    <row r="168" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A168" s="3"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -5040,7 +5151,7 @@
       <c r="G168" s="1"/>
       <c r="H168" s="4"/>
     </row>
-    <row r="169" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A169" s="3"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -5050,7 +5161,7 @@
       <c r="G169" s="1"/>
       <c r="H169" s="4"/>
     </row>
-    <row r="170" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A170" s="3"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -5060,7 +5171,7 @@
       <c r="G170" s="1"/>
       <c r="H170" s="4"/>
     </row>
-    <row r="171" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A171" s="3"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -5070,7 +5181,7 @@
       <c r="G171" s="1"/>
       <c r="H171" s="4"/>
     </row>
-    <row r="172" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A172" s="3"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -5080,7 +5191,7 @@
       <c r="G172" s="1"/>
       <c r="H172" s="4"/>
     </row>
-    <row r="173" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A173" s="3"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -5090,7 +5201,7 @@
       <c r="G173" s="1"/>
       <c r="H173" s="4"/>
     </row>
-    <row r="174" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A174" s="3"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -5100,7 +5211,7 @@
       <c r="G174" s="1"/>
       <c r="H174" s="4"/>
     </row>
-    <row r="175" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A175" s="3"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -5110,7 +5221,7 @@
       <c r="G175" s="1"/>
       <c r="H175" s="4"/>
     </row>
-    <row r="176" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A176" s="3"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -5120,7 +5231,7 @@
       <c r="G176" s="1"/>
       <c r="H176" s="4"/>
     </row>
-    <row r="177" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A177" s="3"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -5130,7 +5241,7 @@
       <c r="G177" s="1"/>
       <c r="H177" s="4"/>
     </row>
-    <row r="178" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A178" s="3"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -5140,7 +5251,7 @@
       <c r="G178" s="1"/>
       <c r="H178" s="4"/>
     </row>
-    <row r="179" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A179" s="3"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -5150,7 +5261,7 @@
       <c r="G179" s="1"/>
       <c r="H179" s="4"/>
     </row>
-    <row r="180" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A180" s="3"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -5160,7 +5271,7 @@
       <c r="G180" s="1"/>
       <c r="H180" s="4"/>
     </row>
-    <row r="181" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A181" s="3"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -5170,7 +5281,7 @@
       <c r="G181" s="1"/>
       <c r="H181" s="4"/>
     </row>
-    <row r="182" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A182" s="3"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -5180,7 +5291,7 @@
       <c r="G182" s="1"/>
       <c r="H182" s="4"/>
     </row>
-    <row r="183" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A183" s="3"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -5190,7 +5301,7 @@
       <c r="G183" s="1"/>
       <c r="H183" s="4"/>
     </row>
-    <row r="184" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A184" s="3"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -5200,7 +5311,7 @@
       <c r="G184" s="1"/>
       <c r="H184" s="4"/>
     </row>
-    <row r="185" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A185" s="3"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -5210,7 +5321,7 @@
       <c r="G185" s="1"/>
       <c r="H185" s="4"/>
     </row>
-    <row r="186" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A186" s="3"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -5220,7 +5331,7 @@
       <c r="G186" s="1"/>
       <c r="H186" s="4"/>
     </row>
-    <row r="187" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A187" s="3"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -5230,7 +5341,7 @@
       <c r="G187" s="1"/>
       <c r="H187" s="4"/>
     </row>
-    <row r="188" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A188" s="3"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -5240,7 +5351,7 @@
       <c r="G188" s="1"/>
       <c r="H188" s="4"/>
     </row>
-    <row r="189" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A189" s="3"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -5250,7 +5361,7 @@
       <c r="G189" s="1"/>
       <c r="H189" s="4"/>
     </row>
-    <row r="190" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A190" s="3"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -5260,7 +5371,7 @@
       <c r="G190" s="1"/>
       <c r="H190" s="4"/>
     </row>
-    <row r="191" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A191" s="3"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -5270,7 +5381,7 @@
       <c r="G191" s="1"/>
       <c r="H191" s="4"/>
     </row>
-    <row r="192" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A192" s="3"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -5280,7 +5391,7 @@
       <c r="G192" s="1"/>
       <c r="H192" s="4"/>
     </row>
-    <row r="193" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A193" s="3"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -5290,7 +5401,7 @@
       <c r="G193" s="1"/>
       <c r="H193" s="4"/>
     </row>
-    <row r="194" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A194" s="3"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -5300,7 +5411,7 @@
       <c r="G194" s="1"/>
       <c r="H194" s="4"/>
     </row>
-    <row r="195" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A195" s="3"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -5310,7 +5421,7 @@
       <c r="G195" s="1"/>
       <c r="H195" s="4"/>
     </row>
-    <row r="196" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A196" s="3"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -5320,7 +5431,7 @@
       <c r="G196" s="1"/>
       <c r="H196" s="4"/>
     </row>
-    <row r="197" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A197" s="3"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -5330,7 +5441,7 @@
       <c r="G197" s="1"/>
       <c r="H197" s="4"/>
     </row>
-    <row r="198" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A198" s="3"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -5340,7 +5451,7 @@
       <c r="G198" s="1"/>
       <c r="H198" s="4"/>
     </row>
-    <row r="199" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A199" s="3"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -5350,7 +5461,7 @@
       <c r="G199" s="1"/>
       <c r="H199" s="4"/>
     </row>
-    <row r="200" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A200" s="3"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -5360,7 +5471,7 @@
       <c r="G200" s="1"/>
       <c r="H200" s="4"/>
     </row>
-    <row r="201" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A201" s="3"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -5370,7 +5481,7 @@
       <c r="G201" s="1"/>
       <c r="H201" s="4"/>
     </row>
-    <row r="202" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A202" s="3"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -5380,7 +5491,7 @@
       <c r="G202" s="1"/>
       <c r="H202" s="4"/>
     </row>
-    <row r="203" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A203" s="3"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -5390,7 +5501,7 @@
       <c r="G203" s="1"/>
       <c r="H203" s="4"/>
     </row>
-    <row r="204" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A204" s="3"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -5400,7 +5511,7 @@
       <c r="G204" s="1"/>
       <c r="H204" s="4"/>
     </row>
-    <row r="205" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A205" s="3"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -5410,7 +5521,7 @@
       <c r="G205" s="1"/>
       <c r="H205" s="4"/>
     </row>
-    <row r="206" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A206" s="3"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -5420,7 +5531,7 @@
       <c r="G206" s="1"/>
       <c r="H206" s="4"/>
     </row>
-    <row r="207" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A207" s="3"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -5430,7 +5541,7 @@
       <c r="G207" s="1"/>
       <c r="H207" s="4"/>
     </row>
-    <row r="208" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A208" s="3"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -5440,7 +5551,7 @@
       <c r="G208" s="1"/>
       <c r="H208" s="4"/>
     </row>
-    <row r="209" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A209" s="3"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -5450,7 +5561,7 @@
       <c r="G209" s="1"/>
       <c r="H209" s="4"/>
     </row>
-    <row r="210" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A210" s="3"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -5460,7 +5571,7 @@
       <c r="G210" s="1"/>
       <c r="H210" s="4"/>
     </row>
-    <row r="211" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A211" s="3"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -5470,7 +5581,7 @@
       <c r="G211" s="1"/>
       <c r="H211" s="4"/>
     </row>
-    <row r="212" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A212" s="3"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -5480,7 +5591,7 @@
       <c r="G212" s="1"/>
       <c r="H212" s="4"/>
     </row>
-    <row r="213" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A213" s="3"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -5490,7 +5601,7 @@
       <c r="G213" s="1"/>
       <c r="H213" s="4"/>
     </row>
-    <row r="214" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A214" s="3"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -5500,7 +5611,7 @@
       <c r="G214" s="1"/>
       <c r="H214" s="4"/>
     </row>
-    <row r="215" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A215" s="3"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -5510,7 +5621,7 @@
       <c r="G215" s="1"/>
       <c r="H215" s="4"/>
     </row>
-    <row r="216" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:8" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A216" s="3"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -5520,7 +5631,7 @@
       <c r="G216" s="1"/>
       <c r="H216" s="4"/>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="5"/>
       <c r="B217" s="6"/>
       <c r="C217" s="6"/>

</xml_diff>

<commit_message>
MAJ courbe en s
</commit_message>
<xml_diff>
--- a/Gestion/Courbe_en_S.xlsx
+++ b/Gestion/Courbe_en_S.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Semaine</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Progression %</t>
+  </si>
+  <si>
+    <t>*toutes les heures et estimations</t>
+  </si>
+  <si>
+    <t>viennent de trello</t>
   </si>
 </sst>
 </file>
@@ -3157,8 +3163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.1328125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -3562,7 +3568,9 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:16" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="3"/>
+      <c r="A10" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -3572,7 +3580,9 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:16" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A11" s="3"/>
+      <c r="A11" s="19" t="s">
+        <v>25</v>
+      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>

</xml_diff>